<commit_message>
teste da planilha 4
</commit_message>
<xml_diff>
--- a/data/relatorio_efetivados.xlsx
+++ b/data/relatorio_efetivados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
   <si>
     <t>Nome</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Pedro L Sales</t>
-  </si>
-  <si>
     <t>Antonio Raimundo De Carvalho</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Mateus Ávila Viggiano</t>
   </si>
   <si>
-    <t>Maria Alice Maciel Rodrigues</t>
-  </si>
-  <si>
     <t>Eliete De Paiva Ribeiro</t>
   </si>
   <si>
@@ -70,12 +64,6 @@
     <t>Juliane Francisca Campos Silva</t>
   </si>
   <si>
-    <t>Leonardo E Lisboa Da Silva</t>
-  </si>
-  <si>
-    <t>Arthur Henrique Teixeira De Resende</t>
-  </si>
-  <si>
     <t>Edilea Aparecida Soares</t>
   </si>
   <si>
@@ -85,7 +73,70 @@
     <t>Brendha Oliveira Silva</t>
   </si>
   <si>
-    <t>32999981121</t>
+    <t>Eliana Aparecida Reis Santana</t>
+  </si>
+  <si>
+    <t>Fernanda Guimaraes De Andrade</t>
+  </si>
+  <si>
+    <t>Sergio Junior Reis Silva</t>
+  </si>
+  <si>
+    <t>Tiago Conceição Orlando</t>
+  </si>
+  <si>
+    <t>Jordano Castorino Sacramento Martins</t>
+  </si>
+  <si>
+    <t>Samuel Enrico Castro Bruscadin</t>
+  </si>
+  <si>
+    <t>Ana Clara Castro Bruscadin</t>
+  </si>
+  <si>
+    <t>Ítalo Jacques Cruz</t>
+  </si>
+  <si>
+    <t>Leandro Paulo Da Silva</t>
+  </si>
+  <si>
+    <t>Raphaela Amorim De Castro</t>
+  </si>
+  <si>
+    <t>Jéssica Mônica De Carvalho</t>
+  </si>
+  <si>
+    <t>Horades Maria De Sousa</t>
+  </si>
+  <si>
+    <t>João Victor De Andrade</t>
+  </si>
+  <si>
+    <t>Maíra Lusiano</t>
+  </si>
+  <si>
+    <t>Bryan Davi Dias Silva</t>
+  </si>
+  <si>
+    <t>Maria Vitoria Dias Romão</t>
+  </si>
+  <si>
+    <t>Adelaine Trindade Dias</t>
+  </si>
+  <si>
+    <t>Luzia Da Trindade Silva Lima</t>
+  </si>
+  <si>
+    <t>Wesley Cosme Fernandes</t>
+  </si>
+  <si>
+    <t>Marluz Guimaraes Dos Santos Santos</t>
+  </si>
+  <si>
+    <t>Iara Lucia Aparecida Silva Souza</t>
+  </si>
+  <si>
+    <t>Ana Carolina Grassi</t>
   </si>
   <si>
     <t>32999793008</t>
@@ -103,9 +154,6 @@
     <t>3299139797</t>
   </si>
   <si>
-    <t>32998016899</t>
-  </si>
-  <si>
     <t>32984120630</t>
   </si>
   <si>
@@ -130,12 +178,6 @@
     <t>32984315484</t>
   </si>
   <si>
-    <t>32999224290</t>
-  </si>
-  <si>
-    <t>3299913375</t>
-  </si>
-  <si>
     <t>32998171870</t>
   </si>
   <si>
@@ -145,7 +187,58 @@
     <t>3299180124</t>
   </si>
   <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999981121&amp;text=Ol%C3%A1%20Pedro%20L%20Sales%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+    <t>32984036161</t>
+  </si>
+  <si>
+    <t>32999032442</t>
+  </si>
+  <si>
+    <t>32984120641</t>
+  </si>
+  <si>
+    <t>32999372077</t>
+  </si>
+  <si>
+    <t>32999047509</t>
+  </si>
+  <si>
+    <t>38999351002</t>
+  </si>
+  <si>
+    <t>32999700636</t>
+  </si>
+  <si>
+    <t>32984737490</t>
+  </si>
+  <si>
+    <t>32999455959</t>
+  </si>
+  <si>
+    <t>32999971385</t>
+  </si>
+  <si>
+    <t>32999300754</t>
+  </si>
+  <si>
+    <t>31986078855</t>
+  </si>
+  <si>
+    <t>31985629997</t>
+  </si>
+  <si>
+    <t>32991569146</t>
+  </si>
+  <si>
+    <t>32984938255</t>
+  </si>
+  <si>
+    <t>3299860028</t>
+  </si>
+  <si>
+    <t>32998105854</t>
+  </si>
+  <si>
+    <t>32999198441</t>
   </si>
   <si>
     <t>https://web.whatsapp.com/send?phone=+5532999793008&amp;text=Ol%C3%A1%20Antonio%20Raimundo%20De%20Carvalho%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
@@ -163,9 +256,6 @@
     <t>https://web.whatsapp.com/send?phone=+553299139797&amp;text=Ol%C3%A1%20Mateus%20%C3%81vila%20Viggiano%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
   <si>
-    <t>https://web.whatsapp.com/send?phone=+5532998016899&amp;text=Ol%C3%A1%20Maria%20Alice%20Maciel%20Rodrigues%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
     <t>https://web.whatsapp.com/send?phone=+5532984120630&amp;text=Ol%C3%A1%20Eliete%20De%20Paiva%20Ribeiro%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
   <si>
@@ -190,12 +280,6 @@
     <t>https://web.whatsapp.com/send?phone=+5532984315484&amp;text=Ol%C3%A1%20Juliane%20Francisca%20Campos%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
   <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999224290&amp;text=Ol%C3%A1%20Leonardo%20E%20Lisboa%20Da%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+553299913375&amp;text=Ol%C3%A1%20Arthur%20Henrique%20Teixeira%20De%20Resende%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
     <t>https://web.whatsapp.com/send?phone=+5532998171870&amp;text=Ol%C3%A1%20Edilea%20Aparecida%20Soares%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
   <si>
@@ -203,6 +287,72 @@
   </si>
   <si>
     <t>https://web.whatsapp.com/send?phone=+553299180124&amp;text=Ol%C3%A1%20Brendha%20Oliveira%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532984036161&amp;text=Ol%C3%A1%20Eliana%20Aparecida%20Reis%20Santana%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999032442&amp;text=Ol%C3%A1%20Fernanda%20Guimaraes%20De%20Andrade%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532984120641&amp;text=Ol%C3%A1%20Sergio%20Junior%20Reis%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999372077&amp;text=Ol%C3%A1%20Tiago%20Concei%C3%A7%C3%A3o%20Orlando%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999047509&amp;text=Ol%C3%A1%20Jordano%20Castorino%20Sacramento%20Martins%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5538999351002&amp;text=Ol%C3%A1%20Samuel%20Enrico%20Castro%20Bruscadin%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5538999351002&amp;text=Ol%C3%A1%20Ana%20Clara%20Castro%20Bruscadin%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999700636&amp;text=Ol%C3%A1%20%C3%8Dtalo%20Jacques%20Cruz%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532984737490&amp;text=Ol%C3%A1%20Leandro%20Paulo%20Da%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999455959&amp;text=Ol%C3%A1%20Raphaela%20Amorim%20De%20Castro%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999971385&amp;text=Ol%C3%A1%20J%C3%A9ssica%20M%C3%B4nica%20De%20Carvalho%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999300754&amp;text=Ol%C3%A1%20Horades%20Maria%20De%20Sousa%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5531986078855&amp;text=Ol%C3%A1%20Jo%C3%A3o%20Victor%20De%20Andrade%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5531985629997&amp;text=Ol%C3%A1%20Ma%C3%ADra%20Lusiano%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999372077&amp;text=Ol%C3%A1%20Bryan%20Davi%20Dias%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999372077&amp;text=Ol%C3%A1%20Maria%20Vitoria%20Dias%20Rom%C3%A3o%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999372077&amp;text=Ol%C3%A1%20Adelaine%20Trindade%20Dias%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532991569146&amp;text=Ol%C3%A1%20Luzia%20Da%20Trindade%20Silva%20Lima%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532984938255&amp;text=Ol%C3%A1%20Wesley%20Cosme%20Fernandes%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+553299860028&amp;text=Ol%C3%A1%20Marluz%20Guimaraes%20Dos%20Santos%20Santos%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532998105854&amp;text=Ol%C3%A1%20Iara%20Lucia%20Aparecida%20Silva%20Souza%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
+  </si>
+  <si>
+    <t>https://web.whatsapp.com/send?phone=+5532999198441&amp;text=Ol%C3%A1%20Ana%20Carolina%20Grassi%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
 </sst>
 </file>
@@ -573,7 +723,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,10 +745,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -606,10 +756,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -617,10 +767,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -628,10 +778,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -639,10 +789,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -650,10 +800,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -661,10 +811,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -672,10 +822,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -683,10 +833,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -694,10 +844,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -705,10 +855,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -716,10 +866,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -727,10 +877,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -738,10 +888,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -749,10 +899,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -760,10 +910,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -771,10 +921,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -782,10 +932,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -793,10 +943,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -804,10 +954,208 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
         <v>62</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -832,6 +1180,24 @@
     <hyperlink ref="C19" r:id="rId18"/>
     <hyperlink ref="C20" r:id="rId19"/>
     <hyperlink ref="C21" r:id="rId20"/>
+    <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C36" r:id="rId35"/>
+    <hyperlink ref="C37" r:id="rId36"/>
+    <hyperlink ref="C38" r:id="rId37"/>
+    <hyperlink ref="C39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
teste da planilha 5
</commit_message>
<xml_diff>
--- a/data/relatorio_efetivados.xlsx
+++ b/data/relatorio_efetivados.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Nome</t>
   </si>
@@ -25,54 +25,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Antonio Raimundo De Carvalho</t>
-  </si>
-  <si>
-    <t>Juaguaci Corrêa De Araújo Monsores</t>
-  </si>
-  <si>
-    <t>Tatiane Da Glória Araújo</t>
-  </si>
-  <si>
-    <t>Joao Victor Guimaraes Pinto</t>
-  </si>
-  <si>
-    <t>Mateus Ávila Viggiano</t>
-  </si>
-  <si>
-    <t>Eliete De Paiva Ribeiro</t>
-  </si>
-  <si>
-    <t>Joice Coutinho De Souza</t>
-  </si>
-  <si>
-    <t>Bruna Carolina Da Silva</t>
-  </si>
-  <si>
-    <t>Luciana Araujo Dos Reis</t>
-  </si>
-  <si>
-    <t>Jose Cardoso Rodrigues</t>
-  </si>
-  <si>
-    <t>Crisvaldo Alves De Carvalho</t>
-  </si>
-  <si>
-    <t>Sarah Botega Dos Santos</t>
-  </si>
-  <si>
-    <t>Juliane Francisca Campos Silva</t>
-  </si>
-  <si>
-    <t>Edilea Aparecida Soares</t>
-  </si>
-  <si>
-    <t>Walysson Bruno Marcelino</t>
-  </si>
-  <si>
-    <t>Brendha Oliveira Silva</t>
-  </si>
-  <si>
     <t>Eliana Aparecida Reis Santana</t>
   </si>
   <si>
@@ -139,54 +91,6 @@
     <t>Ana Carolina Grassi</t>
   </si>
   <si>
-    <t>32999793008</t>
-  </si>
-  <si>
-    <t>32999923860</t>
-  </si>
-  <si>
-    <t>32999839001</t>
-  </si>
-  <si>
-    <t>32998231263</t>
-  </si>
-  <si>
-    <t>3299139797</t>
-  </si>
-  <si>
-    <t>32984120630</t>
-  </si>
-  <si>
-    <t>32999790209</t>
-  </si>
-  <si>
-    <t>32998538983</t>
-  </si>
-  <si>
-    <t>24998179339</t>
-  </si>
-  <si>
-    <t>32998130056</t>
-  </si>
-  <si>
-    <t>32984444450</t>
-  </si>
-  <si>
-    <t>32985011047</t>
-  </si>
-  <si>
-    <t>32984315484</t>
-  </si>
-  <si>
-    <t>32998171870</t>
-  </si>
-  <si>
-    <t>32984193044</t>
-  </si>
-  <si>
-    <t>3299180124</t>
-  </si>
-  <si>
     <t>32984036161</t>
   </si>
   <si>
@@ -239,54 +143,6 @@
   </si>
   <si>
     <t>32999198441</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999793008&amp;text=Ol%C3%A1%20Antonio%20Raimundo%20De%20Carvalho%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999923860&amp;text=Ol%C3%A1%20Juaguaci%20Corr%C3%AAa%20De%20Ara%C3%BAjo%20Monsores%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999839001&amp;text=Ol%C3%A1%20Tatiane%20Da%20Gl%C3%B3ria%20Ara%C3%BAjo%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532998231263&amp;text=Ol%C3%A1%20Joao%20Victor%20Guimaraes%20Pinto%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+553299139797&amp;text=Ol%C3%A1%20Mateus%20%C3%81vila%20Viggiano%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532984120630&amp;text=Ol%C3%A1%20Eliete%20De%20Paiva%20Ribeiro%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532999790209&amp;text=Ol%C3%A1%20Joice%20Coutinho%20De%20Souza%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532998538983&amp;text=Ol%C3%A1%20Bruna%20Carolina%20Da%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5524998179339&amp;text=Ol%C3%A1%20Luciana%20Araujo%20Dos%20Reis%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532998130056&amp;text=Ol%C3%A1%20Jose%20Cardoso%20Rodrigues%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532984444450&amp;text=Ol%C3%A1%20Crisvaldo%20Alves%20De%20Carvalho%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532985011047&amp;text=Ol%C3%A1%20Sarah%20Botega%20Dos%20Santos%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532984315484&amp;text=Ol%C3%A1%20Juliane%20Francisca%20Campos%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532998171870&amp;text=Ol%C3%A1%20Edilea%20Aparecida%20Soares%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+5532984193044&amp;text=Ol%C3%A1%20Walysson%20Bruno%20Marcelino%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
-  </si>
-  <si>
-    <t>https://web.whatsapp.com/send?phone=+553299180124&amp;text=Ol%C3%A1%20Brendha%20Oliveira%20Silva%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
   </si>
   <si>
     <t>https://web.whatsapp.com/send?phone=+5532984036161&amp;text=Ol%C3%A1%20Eliana%20Aparecida%20Reis%20Santana%20Tudo%20bem%3F%F0%9F%98%8A%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0APassando%20para%20relembrar%20o%20or%C3%A7amento%20que%20voc%C3%AA%20fez%20conosco%20%F0%9F%92%AC%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AEstamos%20com%20%C3%B3timas%20condi%C3%A7%C3%B5es%20para%20te%20ajudar%20a%20iniciar%20seu%20tratamento%20%F0%9F%92%99%0A%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%20%0AQuer%20entender%20melhor%3F%20Aproveita%20esse%20momento%20para%20garantir%20o%20cuidado%20que%20voc%C3%AA%20merece%21%F0%9F%98%89</t>
@@ -723,7 +579,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -745,10 +601,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -756,10 +612,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -767,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -778,10 +634,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -789,10 +645,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -800,10 +656,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -811,10 +667,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -822,10 +678,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -833,10 +689,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -844,10 +700,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>84</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -855,10 +711,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>85</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -866,10 +722,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -877,10 +733,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -888,10 +744,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -899,10 +755,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -910,10 +766,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -921,10 +777,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -932,10 +788,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -943,10 +799,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -954,10 +810,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -965,10 +821,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -976,186 +832,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
         <v>64</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1182,22 +862,6 @@
     <hyperlink ref="C21" r:id="rId20"/>
     <hyperlink ref="C22" r:id="rId21"/>
     <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
-    <hyperlink ref="C32" r:id="rId31"/>
-    <hyperlink ref="C33" r:id="rId32"/>
-    <hyperlink ref="C34" r:id="rId33"/>
-    <hyperlink ref="C35" r:id="rId34"/>
-    <hyperlink ref="C36" r:id="rId35"/>
-    <hyperlink ref="C37" r:id="rId36"/>
-    <hyperlink ref="C38" r:id="rId37"/>
-    <hyperlink ref="C39" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>